<commit_message>
Changed AIBS2019 file name to AIBS2018 to reflect AIBS-reported release date of the data i.e. June/October 2018.
</commit_message>
<xml_diff>
--- a/metadata/dataset_metadata.xlsx
+++ b/metadata/dataset_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhrey\DOCUME~1\MobaXterm\slash\RemoteFiles\133144_3_0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhrey\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47261348-5049-4EFF-9B48-90C89A276E8A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46DC9603-10BD-4202-9E50-98FA08EA6FB5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5856" activeTab="1" xr2:uid="{5B1D3AE3-0636-4016-8003-3A344A64CD4A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{5B1D3AE3-0636-4016-8003-3A344A64CD4A}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnDescriptions" sheetId="2" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -144,9 +145,6 @@
     <t>NA</t>
   </si>
   <si>
-    <t>AIBS2018</t>
-  </si>
-  <si>
     <t>ctd_ABI.rda</t>
   </si>
   <si>
@@ -204,9 +202,6 @@
     <t>S1_cortex;CA1_hippocampus;hypothalamus;striatum;midbrain</t>
   </si>
   <si>
-    <t>AIBS2019</t>
-  </si>
-  <si>
     <t>original_filename</t>
   </si>
   <si>
@@ -304,13 +299,19 @@
   </si>
   <si>
     <t>L5_All.loom</t>
+  </si>
+  <si>
+    <t>AIBS2017_MTG</t>
+  </si>
+  <si>
+    <t>AIBS2018_MTG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -691,21 +692,21 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="53.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -713,7 +714,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -721,7 +722,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -729,7 +730,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -737,7 +738,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -745,7 +746,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -753,7 +754,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -761,7 +762,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -769,15 +770,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
         <v>34</v>
       </c>
@@ -785,7 +786,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
         <v>29</v>
       </c>
@@ -793,7 +794,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
         <v>30</v>
       </c>
@@ -801,15 +802,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B14" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -828,10 +829,10 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
@@ -847,7 +848,7 @@
     <col min="14" max="14" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -873,7 +874,7 @@
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>34</v>
@@ -885,16 +886,16 @@
         <v>30</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -911,13 +912,13 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I2" t="s">
         <v>36</v>
@@ -932,7 +933,7 @@
         <v>47</v>
       </c>
       <c r="M2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="N2" t="s">
         <v>12</v>
@@ -941,7 +942,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -958,13 +959,13 @@
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I3" t="s">
         <v>36</v>
@@ -979,21 +980,21 @@
         <v>149</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="N3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>89</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
         <v>36</v>
@@ -1002,16 +1003,16 @@
         <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I4">
         <v>3</v>
@@ -1026,39 +1027,39 @@
         <v>36</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5">
         <v>2017</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I5">
         <v>5</v>
@@ -1073,39 +1074,39 @@
         <v>15</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="N5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6">
         <v>2017</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I6" t="s">
         <v>36</v>
@@ -1120,21 +1121,21 @@
         <v>22</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="N6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
         <v>36</v>
@@ -1143,16 +1144,16 @@
         <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I7">
         <v>8</v>
@@ -1167,7 +1168,7 @@
         <v>75</v>
       </c>
       <c r="M7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N7" t="s">
         <v>36</v>
@@ -1176,30 +1177,30 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8">
         <v>2016</v>
       </c>
       <c r="D8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I8" t="s">
         <v>36</v>
@@ -1214,39 +1215,39 @@
         <v>29</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="N8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="O8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C9">
         <v>2016</v>
       </c>
       <c r="D9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I9" t="s">
         <v>36</v>
@@ -1261,39 +1262,39 @@
         <v>49</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="N9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="O9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C10">
         <v>2018</v>
       </c>
       <c r="D10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" t="s">
+        <v>80</v>
+      </c>
+      <c r="G10" t="s">
+        <v>52</v>
+      </c>
+      <c r="H10" t="s">
         <v>79</v>
-      </c>
-      <c r="E10" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" t="s">
-        <v>82</v>
-      </c>
-      <c r="G10" t="s">
-        <v>53</v>
-      </c>
-      <c r="H10" t="s">
-        <v>81</v>
       </c>
       <c r="I10">
         <v>3</v>
@@ -1309,39 +1310,39 @@
         <v>36</v>
       </c>
       <c r="M10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="N10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="O10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C11">
         <v>2018</v>
       </c>
       <c r="D11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I11" t="s">
         <v>36</v>
@@ -1357,18 +1358,18 @@
         <v>36</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="N11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="O11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
@@ -1377,19 +1378,19 @@
         <v>2018</v>
       </c>
       <c r="D12" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I12" t="s">
         <v>36</v>
@@ -1404,10 +1405,10 @@
         <v>114</v>
       </c>
       <c r="M12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="N12" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="O12" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Updated specificity matrix from Agarwal 2020
</commit_message>
<xml_diff>
--- a/metadata/dataset_metadata.xlsx
+++ b/metadata/dataset_metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhrey\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46DC9603-10BD-4202-9E50-98FA08EA6FB5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DD16E3-4134-46D1-9593-AC8EB1DAC891}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{5B1D3AE3-0636-4016-8003-3A344A64CD4A}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="98">
   <si>
     <t>resource_name</t>
   </si>
@@ -305,6 +305,27 @@
   </si>
   <si>
     <t>AIBS2018_MTG</t>
+  </si>
+  <si>
+    <t>Agarwal</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE140231</t>
+  </si>
+  <si>
+    <t>GSE140231_RAW.tar</t>
+  </si>
+  <si>
+    <t>Agarwal2020_SNIG</t>
+  </si>
+  <si>
+    <t>cortex</t>
+  </si>
+  <si>
+    <t>substantia_nigra</t>
+  </si>
+  <si>
+    <t>Agarwal2020_CRTX</t>
   </si>
 </sst>
 </file>
@@ -826,10 +847,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{351338E7-7D5C-4ED0-A47D-F929A168C2CA}">
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1414,6 +1435,100 @@
         <v>17</v>
       </c>
     </row>
+    <row r="13" spans="1:15">
+      <c r="A13" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13">
+        <v>2020</v>
+      </c>
+      <c r="D13" t="s">
+        <v>92</v>
+      </c>
+      <c r="E13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" t="s">
+        <v>96</v>
+      </c>
+      <c r="G13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13" t="s">
+        <v>46</v>
+      </c>
+      <c r="I13">
+        <v>5</v>
+      </c>
+      <c r="J13">
+        <v>6105</v>
+      </c>
+      <c r="K13">
+        <v>7</v>
+      </c>
+      <c r="L13">
+        <v>10</v>
+      </c>
+      <c r="M13" t="s">
+        <v>92</v>
+      </c>
+      <c r="N13" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="O13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14">
+        <v>2020</v>
+      </c>
+      <c r="D14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G14" t="s">
+        <v>52</v>
+      </c>
+      <c r="H14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I14">
+        <v>5</v>
+      </c>
+      <c r="J14">
+        <v>12015</v>
+      </c>
+      <c r="K14">
+        <v>6</v>
+      </c>
+      <c r="L14">
+        <v>23</v>
+      </c>
+      <c r="M14" t="s">
+        <v>92</v>
+      </c>
+      <c r="N14" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="O14" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{93819ACF-86E3-4A59-BE22-EDBCF5B7F5FE}"/>

</xml_diff>

<commit_message>
Updated documentation after running devtools::check()
</commit_message>
<xml_diff>
--- a/metadata/dataset_metadata.xlsx
+++ b/metadata/dataset_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhrey\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhrey\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{224E46B3-AAF1-4F85-A06D-4CD2848372E0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B41E6B7-B21B-45F0-B55F-91BD4EEB7232}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{5B1D3AE3-0636-4016-8003-3A344A64CD4A}"/>
+    <workbookView xWindow="28680" yWindow="-1065" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5B1D3AE3-0636-4016-8003-3A344A64CD4A}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnDescriptions" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="115">
   <si>
     <t>resource_name</t>
   </si>
@@ -139,9 +141,6 @@
     <t>NA</t>
   </si>
   <si>
-    <t>ctd_ABI.rda</t>
-  </si>
-  <si>
     <t>ctd_allKI.rda</t>
   </si>
   <si>
@@ -151,9 +150,6 @@
     <t>Unpublished</t>
   </si>
   <si>
-    <t>http://celltypes.brain-map.org/rnaseq</t>
-  </si>
-  <si>
     <t>Habib</t>
   </si>
   <si>
@@ -295,9 +291,6 @@
     <t>L5_All.loom</t>
   </si>
   <si>
-    <t>AIBS2017_MTG</t>
-  </si>
-  <si>
     <t>AIBS2018_MTG</t>
   </si>
   <si>
@@ -383,6 +376,9 @@
   </si>
   <si>
     <t>adipose tissue;adrenal gland;blood;blood vessel;brain - amygdala;brain - anterior cingulate cortex (ba24);brain - caudate (basal ganglia);brain - cerebellar hemisphere;brain - cerebellum;brain - cortex;brain - frontal cortex (ba9);brain - hippocampus;brain - hypothalamus;brain - nucleus accumbens (basal ganglia);brain - putamen (basal ganglia);brain - spinal cord (cervical c-1);brain - substantia nigra;breast;colon;esophagus;heart;liver;lung;muscle;nerve;ovary;pancreas;pituitary;prostate;salivary gland;skin;small intestine;spleen;stomach;thyroid;uterus;vagina</t>
+  </si>
+  <si>
+    <t>https://www.nature.com/articles/s41467-020-17876-0</t>
   </si>
 </sst>
 </file>
@@ -788,10 +784,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -863,7 +859,7 @@
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -892,7 +888,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B14" t="s">
         <v>26</v>
@@ -900,10 +896,10 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B15" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -914,10 +910,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{351338E7-7D5C-4ED0-A47D-F929A168C2CA}">
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -962,7 +958,7 @@
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>32</v>
@@ -974,13 +970,13 @@
         <v>28</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -1000,13 +996,13 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I2" t="s">
         <v>34</v>
@@ -1021,7 +1017,7 @@
         <v>47</v>
       </c>
       <c r="M2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="N2" t="s">
         <v>12</v>
@@ -1047,13 +1043,13 @@
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I3" t="s">
         <v>34</v>
@@ -1068,10 +1064,10 @@
         <v>149</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O3" t="s">
         <v>16</v>
@@ -1079,46 +1075,46 @@
     </row>
     <row r="4" spans="1:15">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
         <v>38</v>
       </c>
-      <c r="C4" t="s">
-        <v>34</v>
+      <c r="C4">
+        <v>2017</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F4" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="G4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J4">
-        <v>4401</v>
+        <v>19550</v>
       </c>
       <c r="K4" s="2">
-        <v>6</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>39</v>
+        <v>10</v>
+      </c>
+      <c r="L4" s="2">
+        <v>15</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="N4" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="O4" t="s">
         <v>16</v>
@@ -1129,43 +1125,43 @@
         <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C5">
         <v>2017</v>
       </c>
       <c r="D5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H5" t="s">
         <v>42</v>
       </c>
-      <c r="E5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" t="s">
-        <v>52</v>
-      </c>
-      <c r="G5" t="s">
-        <v>50</v>
-      </c>
-      <c r="H5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I5">
-        <v>5</v>
+      <c r="I5" t="s">
+        <v>34</v>
       </c>
       <c r="J5">
-        <v>19550</v>
+        <v>19561</v>
       </c>
       <c r="K5" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L5" s="2">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O5" t="s">
         <v>16</v>
@@ -1173,46 +1169,46 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>85</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6">
-        <v>2017</v>
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
       </c>
       <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" t="s">
         <v>42</v>
       </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" t="s">
-        <v>52</v>
-      </c>
-      <c r="G6" t="s">
-        <v>68</v>
-      </c>
-      <c r="H6" t="s">
-        <v>44</v>
-      </c>
-      <c r="I6" t="s">
-        <v>34</v>
+      <c r="I6">
+        <v>8</v>
       </c>
       <c r="J6">
-        <v>19561</v>
+        <v>15928</v>
       </c>
       <c r="K6" s="2">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="L6" s="2">
-        <v>22</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>56</v>
+        <v>75</v>
+      </c>
+      <c r="M6" t="s">
+        <v>102</v>
       </c>
       <c r="N6" t="s">
-        <v>49</v>
+        <v>103</v>
       </c>
       <c r="O6" t="s">
         <v>16</v>
@@ -1220,46 +1216,46 @@
     </row>
     <row r="7" spans="1:15">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
         <v>38</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7">
+        <v>2016</v>
+      </c>
+      <c r="D7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" t="s">
         <v>34</v>
       </c>
-      <c r="D7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" t="s">
-        <v>58</v>
-      </c>
-      <c r="G7" t="s">
-        <v>50</v>
-      </c>
-      <c r="H7" t="s">
-        <v>44</v>
-      </c>
-      <c r="I7">
-        <v>8</v>
-      </c>
       <c r="J7">
-        <v>15928</v>
-      </c>
-      <c r="K7" s="2">
-        <v>7</v>
-      </c>
-      <c r="L7" s="2">
-        <v>75</v>
-      </c>
-      <c r="M7" t="s">
-        <v>105</v>
+        <v>1402</v>
+      </c>
+      <c r="K7">
+        <v>11</v>
+      </c>
+      <c r="L7">
+        <v>29</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="N7" t="s">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="O7" t="s">
         <v>16</v>
@@ -1267,46 +1263,46 @@
     </row>
     <row r="8" spans="1:15">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="C8">
         <v>2016</v>
       </c>
       <c r="D8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
       </c>
       <c r="F8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G8" t="s">
         <v>65</v>
       </c>
-      <c r="G8" t="s">
-        <v>68</v>
-      </c>
       <c r="H8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I8" t="s">
         <v>34</v>
       </c>
       <c r="J8">
-        <v>1402</v>
+        <v>1679</v>
       </c>
       <c r="K8">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="L8">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O8" t="s">
         <v>16</v>
@@ -1314,94 +1310,95 @@
     </row>
     <row r="9" spans="1:15">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C9">
-        <v>2016</v>
+        <v>2018</v>
       </c>
       <c r="D9" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="F9" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="G9" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="H9" t="s">
-        <v>45</v>
-      </c>
-      <c r="I9" t="s">
+        <v>75</v>
+      </c>
+      <c r="I9">
+        <v>3</v>
+      </c>
+      <c r="J9">
+        <f>466+3227+459+473</f>
+        <v>4625</v>
+      </c>
+      <c r="K9">
+        <v>24</v>
+      </c>
+      <c r="L9" t="s">
         <v>34</v>
       </c>
-      <c r="J9">
-        <v>1679</v>
-      </c>
-      <c r="K9">
-        <v>7</v>
-      </c>
-      <c r="L9">
-        <v>49</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>56</v>
+      <c r="M9" t="s">
+        <v>70</v>
       </c>
       <c r="N9" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="O9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C10">
         <v>2018</v>
       </c>
       <c r="D10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H10" t="s">
-        <v>77</v>
-      </c>
-      <c r="I10">
-        <v>3</v>
+        <v>42</v>
+      </c>
+      <c r="I10" t="s">
+        <v>34</v>
       </c>
       <c r="J10">
-        <f>466+3227+459+473</f>
-        <v>4625</v>
+        <f>17093+10319</f>
+        <v>27412</v>
       </c>
       <c r="K10">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="L10" t="s">
         <v>34</v>
       </c>
-      <c r="M10" t="s">
-        <v>72</v>
+      <c r="M10" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="N10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O10" t="s">
         <v>15</v>
@@ -1409,94 +1406,93 @@
     </row>
     <row r="11" spans="1:15">
       <c r="A11" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B11" t="s">
-        <v>74</v>
+        <v>9</v>
       </c>
       <c r="C11">
         <v>2018</v>
       </c>
       <c r="D11" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="E11" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="G11" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="H11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I11" t="s">
         <v>34</v>
       </c>
-      <c r="J11">
-        <f>17093+10319</f>
-        <v>27412</v>
+      <c r="J11" s="4">
+        <v>95407</v>
       </c>
       <c r="K11">
+        <v>13</v>
+      </c>
+      <c r="L11">
+        <v>114</v>
+      </c>
+      <c r="M11" t="s">
+        <v>83</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="O11" t="s">
         <v>16</v>
-      </c>
-      <c r="L11" t="s">
-        <v>34</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="N11" t="s">
-        <v>71</v>
-      </c>
-      <c r="O11" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:15">
       <c r="A12" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>86</v>
       </c>
       <c r="C12">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="D12" t="s">
-        <v>83</v>
+        <v>114</v>
       </c>
       <c r="E12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" t="s">
+        <v>91</v>
+      </c>
+      <c r="G12" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I12">
+        <v>5</v>
+      </c>
+      <c r="J12">
+        <v>6105</v>
+      </c>
+      <c r="K12">
+        <v>7</v>
+      </c>
+      <c r="L12">
         <v>10</v>
       </c>
-      <c r="F12" t="s">
-        <v>84</v>
-      </c>
-      <c r="G12" t="s">
-        <v>67</v>
-      </c>
-      <c r="H12" t="s">
-        <v>45</v>
-      </c>
-      <c r="I12" t="s">
-        <v>34</v>
-      </c>
-      <c r="J12" s="4">
-        <v>95407</v>
-      </c>
-      <c r="K12">
-        <v>13</v>
-      </c>
-      <c r="L12">
-        <v>114</v>
-      </c>
       <c r="M12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="N12" s="5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="O12" t="s">
         <v>16</v>
@@ -1507,43 +1503,43 @@
         <v>92</v>
       </c>
       <c r="B13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C13">
         <v>2020</v>
       </c>
       <c r="D13" t="s">
+        <v>114</v>
+      </c>
+      <c r="E13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" t="s">
         <v>90</v>
       </c>
-      <c r="E13" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" t="s">
-        <v>94</v>
-      </c>
       <c r="G13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I13">
         <v>5</v>
       </c>
       <c r="J13">
-        <v>6105</v>
+        <v>12015</v>
       </c>
       <c r="K13">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L13">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="M13" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="N13" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="O13" t="s">
         <v>16</v>
@@ -1551,46 +1547,46 @@
     </row>
     <row r="14" spans="1:15">
       <c r="A14" t="s">
+        <v>93</v>
+      </c>
+      <c r="B14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14">
+        <v>2018</v>
+      </c>
+      <c r="D14" t="s">
         <v>95</v>
       </c>
-      <c r="B14" t="s">
-        <v>89</v>
-      </c>
-      <c r="C14">
-        <v>2020</v>
-      </c>
-      <c r="D14" t="s">
-        <v>90</v>
-      </c>
       <c r="E14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F14" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="G14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J14">
-        <v>12015</v>
+        <v>10319</v>
       </c>
       <c r="K14">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="L14">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M14" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="N14" s="5" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="O14" t="s">
         <v>16</v>
@@ -1598,46 +1594,46 @@
     </row>
     <row r="15" spans="1:15">
       <c r="A15" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B15" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C15">
         <v>2018</v>
       </c>
       <c r="D15" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F15" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="G15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I15">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J15">
-        <v>10319</v>
+        <v>19368</v>
       </c>
       <c r="K15">
         <v>8</v>
       </c>
       <c r="L15">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="M15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="N15" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="O15" t="s">
         <v>16</v>
@@ -1645,105 +1641,57 @@
     </row>
     <row r="16" spans="1:15">
       <c r="A16" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B16" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="C16">
-        <v>2018</v>
+        <v>2015</v>
       </c>
       <c r="D16" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="E16" t="s">
-        <v>37</v>
-      </c>
-      <c r="F16" t="s">
-        <v>104</v>
+        <v>36</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>113</v>
       </c>
       <c r="G16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H16" t="s">
-        <v>44</v>
-      </c>
-      <c r="I16">
-        <v>5</v>
-      </c>
-      <c r="J16">
-        <v>19368</v>
-      </c>
-      <c r="K16">
-        <v>8</v>
-      </c>
-      <c r="L16">
-        <v>28</v>
+        <v>107</v>
+      </c>
+      <c r="I16" t="s">
+        <v>34</v>
+      </c>
+      <c r="J16" t="s">
+        <v>34</v>
+      </c>
+      <c r="K16" t="s">
+        <v>34</v>
+      </c>
+      <c r="L16" t="s">
+        <v>34</v>
       </c>
       <c r="M16" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="N16" s="5" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="O16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15">
-      <c r="A17" t="s">
-        <v>108</v>
-      </c>
-      <c r="B17" t="s">
-        <v>107</v>
-      </c>
-      <c r="C17">
-        <v>2015</v>
-      </c>
-      <c r="D17" t="s">
-        <v>109</v>
-      </c>
-      <c r="E17" t="s">
-        <v>37</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="G17" t="s">
-        <v>50</v>
-      </c>
-      <c r="H17" t="s">
-        <v>110</v>
-      </c>
-      <c r="I17" t="s">
-        <v>34</v>
-      </c>
-      <c r="J17" t="s">
-        <v>34</v>
-      </c>
-      <c r="K17" t="s">
-        <v>34</v>
-      </c>
-      <c r="L17" t="s">
-        <v>34</v>
-      </c>
-      <c r="M17" t="s">
-        <v>111</v>
-      </c>
-      <c r="N17" s="5" t="s">
         <v>112</v>
-      </c>
-      <c r="O17" t="s">
-        <v>115</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{93819ACF-86E3-4A59-BE22-EDBCF5B7F5FE}"/>
-    <hyperlink ref="M11" r:id="rId2" location="Derived" xr:uid="{DE6063CE-0FAF-44EF-97FA-A516EA2DB353}"/>
-    <hyperlink ref="M4" r:id="rId3" xr:uid="{98195177-A84C-4D36-8896-9E9325BC95B3}"/>
+    <hyperlink ref="M10" r:id="rId2" location="Derived" xr:uid="{DE6063CE-0FAF-44EF-97FA-A516EA2DB353}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>